<commit_message>
Modified project structure & Added rule engine for different use cases
</commit_message>
<xml_diff>
--- a/src/main/resources/admission.xlsx
+++ b/src/main/resources/admission.xlsx
@@ -22,10 +22,10 @@
     <t>Import</t>
   </si>
   <si>
-    <t>com.admission.drools.api.Student</t>
-  </si>
-  <si>
-    <t>com.admission.drools.api.StudentIdGenerator</t>
+    <t>com.admission.drools.api.model.Student</t>
+  </si>
+  <si>
+    <t>com.admission.drools.api.utilities.StudentIdGenerator</t>
   </si>
   <si>
     <t>RuleTable DiscountCalculation</t>
@@ -118,6 +118,8 @@
     </font>
     <font>
       <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>

</xml_diff>